<commit_message>
alternatives added to output.xlsx
</commit_message>
<xml_diff>
--- a/PythonScheduler/ClassRoom.xlsx
+++ b/PythonScheduler/ClassRoom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhijit Dutt\Documents\UMBC\CMSC_447\Project\meetingMinutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parul\Desktop\UMBC\semester 8\447\Project\GitV\PythonScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A7244D-3886-4E2D-83DE-C41DAE03C718}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230DD11C-3D24-4AB1-A492-5AE0395E43AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4215" yWindow="1320" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="3" r:id="rId1"/>
@@ -762,20 +762,20 @@
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="19.36328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.81640625" style="1" hidden="1"/>
+    <col min="1" max="1" width="10.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.85546875" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -801,7 +801,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -824,7 +824,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -847,7 +847,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -870,7 +870,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -893,7 +893,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -916,7 +916,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -939,7 +939,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -962,7 +962,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -985,7 +985,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>7</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>7</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>7</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>7</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>7</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>7</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>7</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>7</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>7</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>7</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>7</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>7</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>7</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>7</v>
       </c>
@@ -2689,17 +2689,17 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
-    <col min="3" max="16384" width="10.81640625" hidden="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="16384" width="10.85546875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>120</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>110</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>108</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>117</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>112</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>119</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>109</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>114</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>116</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>115</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>113</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>111</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>118</v>
       </c>
@@ -2803,21 +2803,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35"/>
-    <row r="17" x14ac:dyDescent="0.35"/>
-    <row r="18" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="19" x14ac:dyDescent="0.35"/>
-    <row r="20" x14ac:dyDescent="0.35"/>
-    <row r="21" x14ac:dyDescent="0.35"/>
-    <row r="22" x14ac:dyDescent="0.35"/>
-    <row r="23" x14ac:dyDescent="0.35"/>
-    <row r="24" x14ac:dyDescent="0.35"/>
-    <row r="25" x14ac:dyDescent="0.35"/>
-    <row r="26" x14ac:dyDescent="0.35"/>
-    <row r="27" x14ac:dyDescent="0.35"/>
-    <row r="28" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="17" x14ac:dyDescent="0.25"/>
+    <row r="18" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="19" x14ac:dyDescent="0.25"/>
+    <row r="20" x14ac:dyDescent="0.25"/>
+    <row r="21" x14ac:dyDescent="0.25"/>
+    <row r="22" x14ac:dyDescent="0.25"/>
+    <row r="23" x14ac:dyDescent="0.25"/>
+    <row r="24" x14ac:dyDescent="0.25"/>
+    <row r="25" x14ac:dyDescent="0.25"/>
+    <row r="26" x14ac:dyDescent="0.25"/>
+    <row r="27" x14ac:dyDescent="0.25"/>
+    <row r="28" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
     <sortCondition descending="1" ref="B2:B17"/>

</xml_diff>

<commit_message>
adding weight function need to fix 684 error
</commit_message>
<xml_diff>
--- a/PythonScheduler/ClassRoom.xlsx
+++ b/PythonScheduler/ClassRoom.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kayajae/Desktop/447Proj-anna_branch/PythonScheduler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parul\Desktop\UMBC\semester 8\447\Project\GitV\PythonScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C355B0E-C4B9-4CCC-9C8D-6C9598AAD826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26600" windowHeight="16480" activeTab="2"/>
+    <workbookView xWindow="2235" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="3" r:id="rId1"/>
@@ -21,18 +22,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="139">
   <si>
     <t>Subject</t>
   </si>
@@ -98,9 +99,6 @@
   </si>
   <si>
     <t>Discrete Structures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMSC </t>
   </si>
   <si>
     <t>Continued Computer Science for Non-Majors</t>
@@ -457,7 +455,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -818,27 +816,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1" hidden="1"/>
+    <col min="1" max="1" width="10.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.85546875" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -861,10 +859,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -878,7 +876,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>9</v>
@@ -887,7 +885,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -901,7 +899,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>10</v>
@@ -910,7 +908,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -924,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>13</v>
@@ -933,7 +931,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -947,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>14</v>
@@ -956,7 +954,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -970,7 +968,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>15</v>
@@ -979,7 +977,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -993,7 +991,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>16</v>
@@ -1002,7 +1000,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1016,7 +1014,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>18</v>
@@ -1025,7 +1023,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1039,7 +1037,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>10</v>
@@ -1048,7 +1046,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1062,7 +1060,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>19</v>
@@ -1071,7 +1069,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1085,7 +1083,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>20</v>
@@ -1094,7 +1092,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1108,7 +1106,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>14</v>
@@ -1117,7 +1115,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1131,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>9</v>
@@ -1140,7 +1138,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1154,7 +1152,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>10</v>
@@ -1163,7 +1161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -1177,7 +1175,7 @@
         <v>3</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>18</v>
@@ -1186,7 +1184,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1200,7 +1198,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>15</v>
@@ -1209,7 +1207,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1223,7 +1221,7 @@
         <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>14</v>
@@ -1232,7 +1230,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1246,7 +1244,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>13</v>
@@ -1255,30 +1253,30 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B19" s="5">
         <v>291</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="H19" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -1286,13 +1284,13 @@
         <v>304</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20" s="6">
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>9</v>
@@ -1301,7 +1299,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1309,22 +1307,22 @@
         <v>304</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="6">
         <v>2</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H21" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1332,13 +1330,13 @@
         <v>304</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22" s="6">
         <v>3</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>10</v>
@@ -1347,7 +1345,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1355,22 +1353,22 @@
         <v>304</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="6">
         <v>4</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H23" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1378,13 +1376,13 @@
         <v>304</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E24" s="6">
         <v>5</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>9</v>
@@ -1393,7 +1391,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -1401,13 +1399,13 @@
         <v>304</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E25" s="6">
         <v>6</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>10</v>
@@ -1416,7 +1414,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1424,13 +1422,13 @@
         <v>313</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E26" s="6">
         <v>1</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>15</v>
@@ -1439,7 +1437,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -1447,13 +1445,13 @@
         <v>313</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E27" s="6">
         <v>2</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>20</v>
@@ -1462,7 +1460,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -1470,13 +1468,13 @@
         <v>313</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" s="6">
         <v>3</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>14</v>
@@ -1485,7 +1483,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
@@ -1493,13 +1491,13 @@
         <v>313</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E29" s="6">
         <v>4</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>13</v>
@@ -1508,7 +1506,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -1516,13 +1514,13 @@
         <v>331</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="6">
         <v>1</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>18</v>
@@ -1531,7 +1529,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -1539,22 +1537,22 @@
         <v>331</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E31" s="6">
         <v>2</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H31" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -1562,13 +1560,13 @@
         <v>331</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E32" s="6">
         <v>3</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>14</v>
@@ -1577,7 +1575,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -1585,13 +1583,13 @@
         <v>331</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E33" s="6">
         <v>4</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>20</v>
@@ -1600,7 +1598,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -1608,22 +1606,22 @@
         <v>341</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E34" s="6">
         <v>1</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H34" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -1631,22 +1629,22 @@
         <v>341</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E35" s="6">
         <v>2</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H35" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -1654,13 +1652,13 @@
         <v>341</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E36" s="6">
         <v>3</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>19</v>
@@ -1669,7 +1667,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -1677,13 +1675,13 @@
         <v>341</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E37" s="6">
         <v>4</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>14</v>
@@ -1692,7 +1690,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
@@ -1700,13 +1698,13 @@
         <v>341</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E38" s="6">
         <v>5</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>13</v>
@@ -1715,7 +1713,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
@@ -1723,13 +1721,13 @@
         <v>341</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E39" s="6">
         <v>6</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>16</v>
@@ -1738,21 +1736,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="E40" s="6">
         <v>1</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>19</v>
@@ -1761,21 +1759,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E41" s="6">
         <v>1</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>14</v>
@@ -1784,21 +1782,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E42" s="6">
         <v>2</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>13</v>
@@ -1807,21 +1805,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E43" s="6">
         <v>3</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>9</v>
@@ -1830,7 +1828,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
@@ -1838,13 +1836,13 @@
         <v>421</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E44" s="6">
         <v>1</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>15</v>
@@ -1853,7 +1851,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
@@ -1861,13 +1859,13 @@
         <v>421</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E45" s="6">
         <v>2</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>19</v>
@@ -1876,7 +1874,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -1884,13 +1882,13 @@
         <v>421</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E46" s="6">
         <v>3</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>10</v>
@@ -1899,7 +1897,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
@@ -1907,22 +1905,22 @@
         <v>426</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E47" s="6">
         <v>1</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H47" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -1930,13 +1928,13 @@
         <v>426</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E48" s="6">
         <v>3</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>20</v>
@@ -1945,21 +1943,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E49" s="6">
         <v>1</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>14</v>
@@ -1968,7 +1966,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -1976,22 +1974,22 @@
         <v>441</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E50" s="6">
         <v>1</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H50" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -1999,13 +1997,13 @@
         <v>441</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E51" s="6">
         <v>2</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>18</v>
@@ -2014,7 +2012,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -2022,36 +2020,36 @@
         <v>441</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E52" s="6">
         <v>3</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H52" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E53" s="6">
         <v>1</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>18</v>
@@ -2060,7 +2058,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
@@ -2068,13 +2066,13 @@
         <v>447</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E54" s="6">
         <v>1</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G54" s="6" t="s">
         <v>14</v>
@@ -2083,7 +2081,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
@@ -2091,13 +2089,13 @@
         <v>447</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E55" s="6">
         <v>2</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G55" s="6" t="s">
         <v>13</v>
@@ -2106,7 +2104,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -2114,13 +2112,13 @@
         <v>447</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E56" s="6">
         <v>3</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G56" s="6" t="s">
         <v>9</v>
@@ -2129,7 +2127,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -2137,22 +2135,22 @@
         <v>447</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E57" s="6">
         <v>4</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H57" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -2160,13 +2158,13 @@
         <v>455</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E58" s="6">
         <v>2</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>16</v>
@@ -2175,7 +2173,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -2183,13 +2181,13 @@
         <v>461</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E59" s="6">
         <v>1</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G59" s="6" t="s">
         <v>15</v>
@@ -2198,7 +2196,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -2206,13 +2204,13 @@
         <v>461</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E60" s="6">
         <v>2</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G60" s="6" t="s">
         <v>13</v>
@@ -2221,7 +2219,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2229,13 +2227,13 @@
         <v>471</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E61" s="6">
         <v>1</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G61" s="6" t="s">
         <v>16</v>
@@ -2244,7 +2242,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -2252,13 +2250,13 @@
         <v>471</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E62" s="6">
         <v>2</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G62" s="6" t="s">
         <v>20</v>
@@ -2267,7 +2265,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -2275,13 +2273,13 @@
         <v>471</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E63" s="6">
         <v>3</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G63" s="6" t="s">
         <v>10</v>
@@ -2290,21 +2288,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B64" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E64" s="6">
         <v>1</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G64" s="6" t="s">
         <v>14</v>
@@ -2313,7 +2311,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -2321,13 +2319,13 @@
         <v>478</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E65" s="6">
         <v>1</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G65" s="6" t="s">
         <v>15</v>
@@ -2336,21 +2334,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B66" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="E66" s="6">
         <v>1</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G66" s="6" t="s">
         <v>19</v>
@@ -2359,7 +2357,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
@@ -2367,13 +2365,13 @@
         <v>481</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E67" s="6">
         <v>1</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>20</v>
@@ -2382,7 +2380,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>7</v>
       </c>
@@ -2390,36 +2388,36 @@
         <v>691</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E68" s="6">
         <v>1</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H68" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B69" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="E69" s="6">
         <v>1</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G69" s="6" t="s">
         <v>9</v>
@@ -2428,47 +2426,47 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="E70" s="6">
         <v>1</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H70" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B71" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="E71" s="6">
         <v>1</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G71" s="6" t="s">
         <v>10</v>
@@ -2477,24 +2475,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="E72" s="6">
         <v>1</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G72" s="6" t="s">
         <v>20</v>
@@ -2503,7 +2501,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>7</v>
       </c>
@@ -2511,16 +2509,16 @@
         <v>491</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="E73" s="6">
         <v>1</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G73" s="6" t="s">
         <v>16</v>
@@ -2529,7 +2527,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>7</v>
       </c>
@@ -2537,22 +2535,22 @@
         <v>493</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E74" s="6">
         <v>1</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H74" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>7</v>
       </c>
@@ -2560,13 +2558,13 @@
         <v>611</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E75" s="6">
         <v>1</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>20</v>
@@ -2575,7 +2573,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
@@ -2583,22 +2581,22 @@
         <v>621</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E76" s="6">
         <v>1</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H76" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>7</v>
       </c>
@@ -2606,22 +2604,22 @@
         <v>641</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E77" s="6">
         <v>1</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H77" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>7</v>
       </c>
@@ -2629,13 +2627,13 @@
         <v>678</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E78" s="6">
         <v>1</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G78" s="6" t="s">
         <v>19</v>
@@ -2644,7 +2642,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>7</v>
       </c>
@@ -2652,13 +2650,13 @@
         <v>682</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E79" s="6">
         <v>1</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G79" s="6" t="s">
         <v>9</v>
@@ -2667,7 +2665,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
@@ -2675,22 +2673,22 @@
         <v>684</v>
       </c>
       <c r="C80" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E80" s="6">
+        <v>1</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G80" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E80" s="6">
-        <v>1</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="H80" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>7</v>
       </c>
@@ -2698,16 +2696,16 @@
         <v>691</v>
       </c>
       <c r="C81" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="E81" s="6">
         <v>1</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>16</v>
@@ -2716,24 +2714,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E82" s="6">
         <v>1</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G82" s="6" t="s">
         <v>14</v>
@@ -2748,141 +2746,141 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" hidden="1"/>
+    <col min="3" max="16384" width="10.85546875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B13" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2"/>
-    <row r="17" x14ac:dyDescent="0.2"/>
-    <row r="18" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="19" x14ac:dyDescent="0.2"/>
-    <row r="20" x14ac:dyDescent="0.2"/>
-    <row r="21" x14ac:dyDescent="0.2"/>
-    <row r="22" x14ac:dyDescent="0.2"/>
-    <row r="23" x14ac:dyDescent="0.2"/>
-    <row r="24" x14ac:dyDescent="0.2"/>
-    <row r="25" x14ac:dyDescent="0.2"/>
-    <row r="26" x14ac:dyDescent="0.2"/>
-    <row r="27" x14ac:dyDescent="0.2"/>
-    <row r="28" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="17" x14ac:dyDescent="0.25"/>
+    <row r="18" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="19" x14ac:dyDescent="0.25"/>
+    <row r="20" x14ac:dyDescent="0.25"/>
+    <row r="21" x14ac:dyDescent="0.25"/>
+    <row r="22" x14ac:dyDescent="0.25"/>
+    <row r="23" x14ac:dyDescent="0.25"/>
+    <row r="24" x14ac:dyDescent="0.25"/>
+    <row r="25" x14ac:dyDescent="0.25"/>
+    <row r="26" x14ac:dyDescent="0.25"/>
+    <row r="27" x14ac:dyDescent="0.25"/>
+    <row r="28" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState ref="A2:B17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
     <sortCondition descending="1" ref="B2:B17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2890,34 +2888,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2">
         <v>39.253003999999997</v>
@@ -2926,9 +2924,9 @@
         <v>-76.713624999999993</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3">
         <v>39.256816999999998</v>
@@ -2937,9 +2935,9 @@
         <v>-76.711589000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4">
         <v>39.255226</v>
@@ -2948,9 +2946,9 @@
         <v>-76.715367000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5">
         <v>39.254835999999997</v>
@@ -2959,9 +2957,9 @@
         <v>-76.712238999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6">
         <v>39.254564000000002</v>
@@ -2970,9 +2968,9 @@
         <v>-76.714027000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7">
         <v>39.255181999999998</v>
@@ -2981,9 +2979,9 @@
         <v>-76.713509999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B8">
         <v>39.253858999999999</v>
@@ -2992,9 +2990,9 @@
         <v>-76.714301000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B9">
         <v>39.253901999999997</v>
@@ -3003,9 +3001,9 @@
         <v>-76.710881000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B10">
         <v>39.253492999999999</v>
@@ -3014,9 +3012,9 @@
         <v>-76.712834000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11">
         <v>39.254826999999999</v>
@@ -3025,9 +3023,9 @@
         <v>-76.711819000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B12">
         <v>39.254106</v>
@@ -3036,9 +3034,9 @@
         <v>-76.712485999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B13">
         <v>39.255065000000002</v>
@@ -3047,9 +3045,9 @@
         <v>-76.713108000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B14">
         <v>39.254519000000002</v>
@@ -3058,9 +3056,9 @@
         <v>-76.709598999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B15">
         <v>39.255243</v>
@@ -3069,9 +3067,9 @@
         <v>-76.709035</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B16">
         <v>39.253579999999999</v>
@@ -3080,9 +3078,9 @@
         <v>-76.713229999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B17">
         <v>39.254387999999999</v>
@@ -3092,7 +3090,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C17">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated scheduler and GUI 5/19/20 4:58PM
</commit_message>
<xml_diff>
--- a/PythonScheduler/ClassRoom.xlsx
+++ b/PythonScheduler/ClassRoom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parul\Desktop\UMBC\semester 8\447\Project\GitV\PythonScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C355B0E-C4B9-4CCC-9C8D-6C9598AAD826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828B12AF-9BA5-4314-8FD2-867323C87D23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6840" yWindow="1485" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="154">
   <si>
     <t>Subject</t>
   </si>
@@ -450,6 +450,51 @@
   </si>
   <si>
     <t xml:space="preserve">Physics </t>
+  </si>
+  <si>
+    <t>ECOM</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>HIST</t>
+  </si>
+  <si>
+    <t>BIOL</t>
+  </si>
+  <si>
+    <t>CMPE</t>
+  </si>
+  <si>
+    <t>ART</t>
+  </si>
+  <si>
+    <t>BTEC</t>
+  </si>
+  <si>
+    <t>MATH</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>PYSC</t>
+  </si>
+  <si>
+    <t>CHEM</t>
+  </si>
+  <si>
+    <t>PHYS</t>
+  </si>
+  <si>
+    <t>POLI</t>
+  </si>
+  <si>
+    <t>STAT</t>
+  </si>
+  <si>
+    <t>ENGL</t>
   </si>
 </sst>
 </file>
@@ -516,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -532,6 +577,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -2889,10 +2935,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2902,7 +2948,7 @@
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>120</v>
       </c>
@@ -2912,8 +2958,11 @@
       <c r="C1" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -2923,8 +2972,11 @@
       <c r="C2">
         <v>-76.713624999999993</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -2934,8 +2986,11 @@
       <c r="C3">
         <v>-76.711589000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>133</v>
       </c>
@@ -2945,8 +3000,11 @@
       <c r="C4">
         <v>-76.715367000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -2956,8 +3014,11 @@
       <c r="C5">
         <v>-76.712238999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -2967,8 +3028,11 @@
       <c r="C6">
         <v>-76.714027000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -2978,8 +3042,11 @@
       <c r="C7">
         <v>-76.713509999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -2989,8 +3056,11 @@
       <c r="C8">
         <v>-76.714301000000006</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -3000,8 +3070,11 @@
       <c r="C9">
         <v>-76.710881000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>128</v>
       </c>
@@ -3011,8 +3084,11 @@
       <c r="C10">
         <v>-76.712834000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -3022,8 +3098,11 @@
       <c r="C11">
         <v>-76.711819000000006</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>129</v>
       </c>
@@ -3033,8 +3112,11 @@
       <c r="C12">
         <v>-76.712485999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>132</v>
       </c>
@@ -3044,8 +3126,11 @@
       <c r="C13">
         <v>-76.713108000000005</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -3055,8 +3140,11 @@
       <c r="C14">
         <v>-76.709598999999997</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -3066,8 +3154,11 @@
       <c r="C15">
         <v>-76.709035</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>127</v>
       </c>
@@ -3077,8 +3168,11 @@
       <c r="C16">
         <v>-76.713229999999996</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>134</v>
       </c>
@@ -3087,6 +3181,9 @@
       </c>
       <c r="C17">
         <v>-76.713317000000004</v>
+      </c>
+      <c r="D17" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3094,5 +3191,6 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>